<commit_message>
MML Work in Progress
Fixed the orientation of the layout in Layout Editor. Associated all the necessary objects with the panel objects. Started experimenting with `Sections` and `Transits`
</commit_message>
<xml_diff>
--- a/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
+++ b/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="MML_sw_config" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -36,64 +36,64 @@
     <t xml:space="preserve">properties</t>
   </si>
   <si>
-    <t xml:space="preserve">SW 1 LH</t>
+    <t xml:space="preserve">SW 1 RH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 part of crossover between track 1 and 2 on left side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH;RelatedSwitch:MML SW 5 LH;RelatedBlock:MML BLK 3 OS}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-MASTER;RelatedSwitch:MML SW 3 RH;RelatedBlock:MML BLK 3 OS}</t>
   </si>
   <si>
     <t xml:space="preserve">SW 2 LH</t>
   </si>
   <si>
-    <t xml:space="preserve">MML Track 1 point for Platform 1 and 2 on left side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH;RelatedBlock:MML BLK 5 OS}</t>
+    <t xml:space="preserve">MML Track 1 part of crossover between track 1 and 2 on ride side of station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-MASTER;RelatedBlock:MML BLK 5 OS;RelatedSwitch:MML SW 6 LH}</t>
   </si>
   <si>
     <t xml:space="preserve">SW 3 RH</t>
   </si>
   <si>
-    <t xml:space="preserve">MML Track 1 point for Platform 1 and 2 on right side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH;RelatedBlock:MML BLK 8 OS}</t>
+    <t xml:space="preserve">MML Track 2 part of crossover between track 1 and 2 on the left side of station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-SLAVE;RelatedBlock:MML BLK 10 OS;RelatedSwitch:MML SW 1 RH}</t>
   </si>
   <si>
     <t xml:space="preserve">SW 4 RH</t>
   </si>
   <si>
-    <t xml:space="preserve">MML Track 1 part of crossover between track 1 and 2 on ride side of station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH;RelatedBlock:MML BLK 10 OS;RelatedSwitch:MML SW 6 RH}</t>
+    <t xml:space="preserve">MML Track 2 platform 1 and 2 switch on left side of the station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH;RelatedBlock:MML BLK 12 OS;RelatedSwitch:MML SW 6 RH}</t>
   </si>
   <si>
     <t xml:space="preserve">SW 5 LH</t>
   </si>
   <si>
-    <t xml:space="preserve">MML Track 2 part of crossover between track 1 and 2 on the left side of station</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH;RelatedSwitch:MML SW 1 LH;RelatedBlock:MML BLK 15 OS}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW 6 RH</t>
+    <t xml:space="preserve">MML Track 2 platform 1 and 2 switch on right side of the station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH;RelatedSwitch:MML SW 1 LH;RelatedBlock:MML BLK 14 OS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 6 LH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 2 part of crossover between track 1 and 2 on ride side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH;RelatedBlock:MML BLK 17 OS;RelatedSwitch:MML SW 4 RH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-SLAVE;RelatedBlock:MML BLK 16 OS;RelatedSwitch:MML SW 4 RH;RelatedSwitch:MML SW 2 LH}</t>
   </si>
   <si>
     <t xml:space="preserve">panel_ind</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 1</t>
+    <t xml:space="preserve">BLK 1</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 first block on left side</t>
@@ -102,25 +102,25 @@
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:Block}</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 2</t>
+    <t xml:space="preserve">BLK 2</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 3 OS</t>
+    <t xml:space="preserve">BLK 3 OS</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 Switch 1</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 1 LH}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 5 OS</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 1 RH}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 5 OS</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 Switch 2</t>
@@ -129,67 +129,58 @@
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 2 LH}</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 6 PF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track Loop Line Platform 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:LPL;SensedObject:Block;XTRA:Platform 1}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 7 PF2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 1 Platform 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:Block;XTRA:Platform 2}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 8 OS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 1 Switch 3</t>
+    <t xml:space="preserve">BLK 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 1 first block on ride side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 first block on left side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 10 OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 Switch 3</t>
   </si>
   <si>
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 3 RH}</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 10 OS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 1 Switch 4</t>
+    <t xml:space="preserve">BLK 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 12 OS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 Switch 4 </t>
   </si>
   <si>
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 4 RH}</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 1 first block on right side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 2 first block on left side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 15 OS</t>
+    <t xml:space="preserve">BLK 13 PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 Platform 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:Block;XTRA:Platform 1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 14 OS</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 2 Switch 5</t>
@@ -198,31 +189,37 @@
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 5 LH}</t>
   </si>
   <si>
-    <t xml:space="preserve">MML BLK 16 PF3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 2 Platform 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:Block;XTRA:Platform 3}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 17 OS</t>
+    <t xml:space="preserve">BLK 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 16 OS</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 2 Switch 6</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 6 RH}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML BLK 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MML Track 2 first block on the right side</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 6 LH}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Track 2 first block on ride side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLK 19 PF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MML Platform 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:LPL;SensedObject:Block;XTRA:Platform 2}</t>
   </si>
 </sst>
 </file>
@@ -515,15 +512,15 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
   </cols>
   <sheetData>
@@ -555,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -569,12 +566,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -583,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -602,7 +599,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>17</v>
@@ -643,11 +640,11 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
@@ -669,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>23</v>
       </c>
@@ -683,7 +680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
@@ -697,7 +694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>28</v>
       </c>
@@ -711,7 +708,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>31</v>
       </c>
@@ -725,7 +722,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>32</v>
       </c>
@@ -739,7 +736,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>35</v>
       </c>
@@ -747,125 +744,125 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="D8" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D10" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>55</v>
       </c>
@@ -876,63 +873,63 @@
         <v>56</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="B18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D19" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="B20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -957,7 +954,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
   </cols>

</xml_diff>

<commit_message>
MML Panel Lights Phase 1
This phase deals with the script to generate the panel lights for MML. This also deals with the kind of information to send the panel board for blocks with switches. In this version every block that is configured to show a panel light is given a light on the panel. Those with switches are given an additional light that indicates the state of the turnout. The idea behind this is to send the Arduino code messages about the state of the entire block using the bits for the lightsthere by giving the Arduino code the following states of information:

- Switch Normal, Block Occupied
- Switch Normal, Block Unoccupied
- Switch Thrown, Block Occupied
- Switch Thrown, Block Unoccupied

The Arduino code will be responsible for configuring the color and the lit status of the lights for this setup based on the two bit of information received.
</commit_message>
<xml_diff>
--- a/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
+++ b/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MML_sw_config" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -220,14 +220,150 @@
   </si>
   <si>
     <t xml:space="preserve">{StationCode:MML;OnTrack:LPL;SensedObject:Block;XTRA:Platform 2}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aspect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 1R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-distant-approach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:DistantApproach}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 2R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-home-diverging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home;Diverging:Right}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 3R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-mainline-starter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 4R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:LSS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:LSS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 6L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Home;Diverging:Left}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 8L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:DistantApproach}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 9R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 22R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 10R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 11R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Starter}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 12R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;Diverging:Left}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 13R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 14L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 15L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;Diverging:Right}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 16L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Starter}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 17L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;Diverging:Left}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 18L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Home}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 19L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 20R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-general</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:LPL;Direction:Right;StationCode:MML}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 21L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:LPL;Direction:Left;StationCode:MML}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -417,8 +553,12 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,11 +652,11 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.46"/>
@@ -644,7 +784,7 @@
       <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
@@ -948,17 +1088,325 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.2"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0.39375" bottom="0.39375" header="0" footer="0"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
IR Aspect Config Updates and Script Updates
</commit_message>
<xml_diff>
--- a/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
+++ b/CMRI_Scripting.jmri/planning/MML_sw_blk_sig_config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -36,31 +36,31 @@
     <t xml:space="preserve">properties</t>
   </si>
   <si>
-    <t xml:space="preserve">SW 1 RH</t>
+    <t xml:space="preserve">SW 1A RH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 part of crossover between track 1 and 2 on left side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-MASTER;RelatedSwitch:MML SW 3 RH;RelatedBlock:MML BLK 3 OS}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW 2 LH</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-MASTER;RelatedSwitch:MML SW 1B RH;RelatedBlock:MML BLK 3 OS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 2A LH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 1 part of crossover between track 1 and 2 on ride side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-MASTER;RelatedBlock:MML BLK 5 OS;RelatedSwitch:MML SW 6 LH}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW 3 RH</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-MASTER;RelatedBlock:MML BLK 5 OS;RelatedSwitch:MML SW 2B LH}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW 1B RH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 2 part of crossover between track 1 and 2 on the left side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-SLAVE;RelatedBlock:MML BLK 10 OS;RelatedSwitch:MML SW 1 RH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:RH-SLAVE;RelatedBlock:MML BLK 10 OS;RelatedSwitch:MML SW 1A RH}</t>
   </si>
   <si>
     <t xml:space="preserve">SW 4 RH</t>
@@ -81,13 +81,13 @@
     <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH;RelatedSwitch:MML SW 1 LH;RelatedBlock:MML BLK 14 OS}</t>
   </si>
   <si>
-    <t xml:space="preserve">SW 6 LH</t>
+    <t xml:space="preserve">SW 2B LH</t>
   </si>
   <si>
     <t xml:space="preserve">MML Track 2 part of crossover between track 1 and 2 on ride side of station</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-SLAVE;RelatedBlock:MML BLK 16 OS;RelatedSwitch:MML SW 4 RH;RelatedSwitch:MML SW 2 LH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SwitchType:LH-SLAVE;RelatedBlock:MML BLK 16 OS;RelatedSwitch:MML SW 2A RH;RelatedSwitch:MML SW 2 LH}</t>
   </si>
   <si>
     <t xml:space="preserve">panel_ind</t>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">MML Track 1 Switch 1</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 1 RH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 1A RH}</t>
   </si>
   <si>
     <t xml:space="preserve">BLK 4</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">MML Track 1 Switch 2</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 2 LH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 2A LH}</t>
   </si>
   <si>
     <t xml:space="preserve">BLK 6</t>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">MML Track 2 Switch 3</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 3 RH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 1B RH}</t>
   </si>
   <si>
     <t xml:space="preserve">BLK 11</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">MML Track 2 Switch 6</t>
   </si>
   <si>
-    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 6 LH}</t>
+    <t xml:space="preserve">{StationCode:MML;OnTrack:MNL;SensedObject:BlockOverSwitch;RelatedObject:MML SW 2B LH}</t>
   </si>
   <si>
     <t xml:space="preserve">BLK 17</t>
@@ -225,133 +225,139 @@
     <t xml:space="preserve">aspect</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 1R</t>
+    <t xml:space="preserve">SG 1R DST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-aspect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:DistantApproach}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 2R HM DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-aspect-with-route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home;Diverging:Right}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 3R MNL CTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-aspect-rg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 4R MNL CTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:LSS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 5L LSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:LSS}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 6L MNL CTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 7L MNL DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Home;Diverging:Left}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 8L DST</t>
   </si>
   <si>
     <t xml:space="preserve">4-distant-approach</t>
   </si>
   <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:DistantApproach}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 2R</t>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:DistantApproach}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 9R HM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-aspect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 22R DST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 10R HM DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 11R MNL STR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Starter}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 12R MNL DV</t>
   </si>
   <si>
     <t xml:space="preserve">3-home-diverging</t>
   </si>
   <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home;Diverging:Right}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 3R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-mainline-starter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 4R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:LSS}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:LSS}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 7L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Home;Diverging:Left}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 8L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:DistantApproach}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 9R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3-home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Home}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 22R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 10R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 11R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;SigType:Starter}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 12R</t>
-  </si>
-  <si>
     <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;Diverging:Left}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 13R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 14L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 15L</t>
+    <t xml:space="preserve">SG 13R LSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 14L MNL LSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 15L MNL DV</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:MNL;Direction:Right;StationCode:MML;Diverging:Right}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 16L</t>
+    <t xml:space="preserve">SG 16L MNL STR</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Starter}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 17L</t>
+    <t xml:space="preserve">SG 17L MNL DV</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;Diverging:Left}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 18L</t>
+    <t xml:space="preserve">SG 18L HM</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:MNL;Direction:Left;StationCode:MML;SigType:Home}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 19L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SG 20R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-general</t>
+    <t xml:space="preserve">SG 19L DST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SG 20R LPL STR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-aspect-ry</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:LPL;Direction:Right;StationCode:MML}</t>
   </si>
   <si>
-    <t xml:space="preserve">SG 21L</t>
+    <t xml:space="preserve">SG 21L LPL STR</t>
   </si>
   <si>
     <t xml:space="preserve">{OnTrack:LPL;Direction:Left;StationCode:MML}</t>
@@ -653,13 +659,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
   </cols>
@@ -781,10 +787,10 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.16"/>
@@ -1094,10 +1100,10 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.2"/>
   </cols>
   <sheetData>
@@ -1133,7 +1139,8 @@
       <c r="B3" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="1" t="b">
+      <c r="C3" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -1147,7 +1154,8 @@
       <c r="B4" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="1" t="b">
+      <c r="C4" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -1183,7 +1191,8 @@
       <c r="B7" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="1" t="b">
+      <c r="C7" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -1197,7 +1206,8 @@
       <c r="B8" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="1" t="b">
+      <c r="C8" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -1209,32 +1219,34 @@
         <v>84</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1" t="b">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="1" t="b">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>68</v>
@@ -1245,12 +1257,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="1" t="b">
+      <c r="C12" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -1259,35 +1272,37 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="1" t="b">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="1" t="b">
+        <v>95</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>74</v>
@@ -1298,7 +1313,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>74</v>
@@ -1310,100 +1325,107 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="1" t="b">
+      <c r="C17" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="1" t="b">
+        <v>88</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="1" t="b">
+      <c r="C19" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="1" t="b">
+        <v>88</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="1" t="b">
+      <c r="C21" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="1" t="b">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="1" t="b">
+      <c r="C23" s="1" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>